<commit_message>
Add refresh button in menu view controller
</commit_message>
<xml_diff>
--- a/basketBallRecorder/spreadsheet.xlsx
+++ b/basketBallRecorder/spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
   <si>
     <t>Isolation</t>
   </si>
@@ -99,6 +99,22 @@
   </si>
   <si>
     <t>High-Low</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA14"/>
+  <dimension ref="A1:CA29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BT3" sqref="BT3"/>
+      <selection activeCell="BO29" sqref="BO29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -973,12 +989,65 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:79">
+      <c r="BO3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:79">
+      <c r="BO4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:79">
+      <c r="BO5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:79">
+      <c r="BO6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:79">
+      <c r="BO7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:79">
+      <c r="BO8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:79">
+      <c r="BO9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:79">
+      <c r="BO10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:79">
+      <c r="BO11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:79">
+      <c r="BO12" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="13" spans="1:79">
       <c r="BB13" s="2"/>
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
       <c r="BE13" s="2"/>
       <c r="BF13" s="2"/>
+      <c r="BO13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:79">
       <c r="BB14" s="2"/>
@@ -986,16 +1055,87 @@
       <c r="BD14" s="2"/>
       <c r="BE14" s="2"/>
       <c r="BF14" s="2"/>
+      <c r="BO14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:79">
+      <c r="BO15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:79">
+      <c r="BO16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="67:67">
+      <c r="BO17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="67:67">
+      <c r="BO18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="67:67">
+      <c r="BO19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="67:67">
+      <c r="BO20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="67:67">
+      <c r="BO21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="67:67">
+      <c r="BO22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="67:67">
+      <c r="BO23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="67:67">
+      <c r="BO24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="67:67">
+      <c r="BO25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="67:67">
+      <c r="BO26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="67:67">
+      <c r="BO27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="67:67">
+      <c r="BO28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="67:67">
+      <c r="BO29" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="BW1:CA1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="BO1:BS1"/>
     <mergeCell ref="AA1:AE1"/>
     <mergeCell ref="BT1:BV1"/>
     <mergeCell ref="B1:F1"/>
@@ -1005,6 +1145,13 @@
     <mergeCell ref="V1:Z1"/>
     <mergeCell ref="BE1:BI1"/>
     <mergeCell ref="BJ1:BN1"/>
+    <mergeCell ref="BW1:CA1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="BO1:BS1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>